<commit_message>
Updating project plan with the finished dates
</commit_message>
<xml_diff>
--- a/Software Deliveries Log/Project Plan.xlsx
+++ b/Software Deliveries Log/Project Plan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC7E32E-7FCA-4E68-8087-A549A1241B09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A2ACEC-76AD-4024-AD7C-7A0118716978}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
     <t>Project Plan</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>Currently working on modifications asked by Eng. Mohamed Ali</t>
+  </si>
+  <si>
+    <t>Complete RTM</t>
   </si>
 </sst>
 </file>
@@ -165,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -184,6 +187,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -274,8 +280,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A4:F8" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A4:F8" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A4:F9" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A4:F9" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Milestone" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Planned Start Date" dataDxfId="4"/>
@@ -788,10 +794,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,7 +876,9 @@
       <c r="D5" s="4">
         <v>43866</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="4">
+        <v>43866</v>
+      </c>
       <c r="F5" s="3" t="s">
         <v>29</v>
       </c>
@@ -888,7 +896,9 @@
       <c r="D6" s="4">
         <v>43866</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="4">
+        <v>43866</v>
+      </c>
       <c r="F6" s="3" t="s">
         <v>29</v>
       </c>
@@ -913,19 +923,37 @@
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B8" s="4">
-        <v>43866</v>
+        <v>43867</v>
       </c>
       <c r="C8" s="4">
-        <v>43866</v>
+        <v>43867</v>
       </c>
       <c r="D8" s="4">
         <v>43867</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="7"/>
       <c r="F8" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="4">
+        <v>43866</v>
+      </c>
+      <c r="C9" s="4">
+        <v>43866</v>
+      </c>
+      <c r="D9" s="4">
+        <v>43867</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>